<commit_message>
Some minor uodate sto BEA_GUI and Global M2.
</commit_message>
<xml_diff>
--- a/Global_M2/Datasums/Top50_DataComp.xlsx
+++ b/Global_M2/Datasums/Top50_DataComp.xlsx
@@ -518,10 +518,10 @@
         <v>45078</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>29921</v>
+        <v>29952</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -555,10 +555,10 @@
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" s="2" t="n">
-        <v>29860</v>
+        <v>29891</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
@@ -596,16 +596,16 @@
         <v>500</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>29860</v>
+        <v>29891</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>29921</v>
+        <v>29952</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -647,10 +647,10 @@
         <v>45078</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>29921</v>
+        <v>29952</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -680,7 +680,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="D6" t="n">
         <v>500</v>
@@ -689,13 +689,13 @@
         <v>31747</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>29921</v>
+        <v>29952</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -737,10 +737,10 @@
         <v>45047</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>29921</v>
+        <v>29952</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -773,19 +773,19 @@
         <v>500</v>
       </c>
       <c r="D8" t="n">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>29860</v>
+        <v>29891</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="G8" s="2" t="n">
         <v>32813</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -821,16 +821,16 @@
         <v>500</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>29860</v>
+        <v>29891</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>29921</v>
+        <v>29952</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -860,22 +860,22 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="D10" t="n">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="E10" s="2" t="n">
         <v>29952</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>30592</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
@@ -911,16 +911,16 @@
         <v>500</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>29830</v>
+        <v>29860</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>45017</v>
+        <v>45047</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>29921</v>
+        <v>29952</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -950,22 +950,22 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D12" t="n">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="E12" s="2" t="n">
         <v>33939</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="G12" s="2" t="n">
         <v>34578</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
@@ -995,7 +995,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="D13" t="n">
         <v>500</v>
@@ -1004,13 +1004,13 @@
         <v>31017</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>29921</v>
+        <v>29952</v>
       </c>
       <c r="H13" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
@@ -1040,22 +1040,22 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="D14" t="n">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="E14" s="2" t="n">
         <v>32325</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="G14" s="2" t="n">
         <v>33239</v>
       </c>
       <c r="H14" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
@@ -1085,7 +1085,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="D15" t="n">
         <v>500</v>
@@ -1094,13 +1094,13 @@
         <v>33543</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="G15" s="2" t="n">
-        <v>29892</v>
+        <v>29921</v>
       </c>
       <c r="H15" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
@@ -1130,22 +1130,22 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="D16" t="n">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="E16" s="2" t="n">
         <v>31382</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="G16" s="2" t="n">
         <v>32813</v>
       </c>
       <c r="H16" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
@@ -1175,22 +1175,22 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D17" t="n">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="E17" s="2" t="n">
         <v>33970</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="G17" s="2" t="n">
         <v>33298</v>
       </c>
       <c r="H17" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
@@ -1226,16 +1226,16 @@
         <v>500</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>29860</v>
+        <v>29891</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>29921</v>
+        <v>29952</v>
       </c>
       <c r="H18" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
@@ -1268,19 +1268,19 @@
         <v>500</v>
       </c>
       <c r="D19" t="n">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>29860</v>
+        <v>29891</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="G19" s="2" t="n">
         <v>33178</v>
       </c>
       <c r="H19" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
@@ -1310,7 +1310,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="D20" t="n">
         <v>500</v>
@@ -1319,13 +1319,13 @@
         <v>25903</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>29921</v>
+        <v>29952</v>
       </c>
       <c r="H20" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
@@ -1355,7 +1355,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D21" t="n">
         <v>500</v>
@@ -1364,13 +1364,13 @@
         <v>35796</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>29921</v>
+        <v>29952</v>
       </c>
       <c r="H21" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
@@ -1400,22 +1400,22 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D22" t="n">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="E22" s="2" t="n">
         <v>35400</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="G22" s="2" t="n">
         <v>34121</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
@@ -1445,22 +1445,22 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D23" t="n">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="E23" s="2" t="n">
         <v>37226</v>
       </c>
       <c r="F23" s="2" t="n">
-        <v>45017</v>
+        <v>45047</v>
       </c>
       <c r="G23" s="2" t="n">
         <v>32965</v>
       </c>
       <c r="H23" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
@@ -1490,22 +1490,22 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D24" t="n">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="E24" s="2" t="n">
         <v>38687</v>
       </c>
       <c r="F24" s="2" t="n">
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="G24" s="2" t="n">
         <v>32813</v>
       </c>
       <c r="H24" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
@@ -1538,19 +1538,19 @@
         <v>500</v>
       </c>
       <c r="D25" t="n">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>29830</v>
+        <v>29860</v>
       </c>
       <c r="F25" s="2" t="n">
-        <v>45017</v>
+        <v>45047</v>
       </c>
       <c r="G25" s="2" t="n">
         <v>35643</v>
       </c>
       <c r="H25" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
@@ -1580,22 +1580,22 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D26" t="n">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E26" s="2" t="n">
         <v>35096</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="G26" s="2" t="n">
         <v>35643</v>
       </c>
       <c r="H26" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
@@ -1631,16 +1631,16 @@
         <v>500</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>29860</v>
+        <v>29891</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="G27" s="2" t="n">
-        <v>29921</v>
+        <v>29952</v>
       </c>
       <c r="H27" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
@@ -1673,7 +1673,7 @@
         <v>500</v>
       </c>
       <c r="D28" t="n">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="E28" s="2" t="n">
         <v>29860</v>
@@ -1685,7 +1685,7 @@
         <v>33725</v>
       </c>
       <c r="H28" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I28" t="inlineStr">
         <is>
@@ -1715,22 +1715,22 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D29" t="n">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E29" s="2" t="n">
         <v>37257</v>
       </c>
       <c r="F29" s="2" t="n">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="G29" s="2" t="n">
         <v>38139</v>
       </c>
       <c r="H29" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I29" t="inlineStr">
         <is>
@@ -1763,19 +1763,19 @@
         <v>500</v>
       </c>
       <c r="D30" t="n">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>29860</v>
+        <v>29891</v>
       </c>
       <c r="F30" s="2" t="n">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="G30" s="2" t="n">
         <v>35339</v>
       </c>
       <c r="H30" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
@@ -1805,7 +1805,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="D31" t="n">
         <v>500</v>
@@ -1814,13 +1814,13 @@
         <v>33239</v>
       </c>
       <c r="F31" s="2" t="n">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="G31" s="2" t="n">
-        <v>29921</v>
+        <v>29952</v>
       </c>
       <c r="H31" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I31" t="inlineStr">
         <is>
@@ -1856,16 +1856,16 @@
         <v>500</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>29860</v>
+        <v>29891</v>
       </c>
       <c r="F32" s="2" t="n">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="G32" s="2" t="n">
-        <v>29921</v>
+        <v>29952</v>
       </c>
       <c r="H32" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I32" t="inlineStr">
         <is>
@@ -1898,7 +1898,7 @@
         <v>450</v>
       </c>
       <c r="D33" t="n">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="E33" s="2" t="n">
         <v>31413</v>
@@ -1910,7 +1910,7 @@
         <v>33178</v>
       </c>
       <c r="H33" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I33" t="inlineStr">
         <is>
@@ -1940,22 +1940,22 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D34" t="n">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E34" s="2" t="n">
         <v>39083</v>
       </c>
       <c r="F34" s="2" t="n">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="G34" s="2" t="n">
         <v>35643</v>
       </c>
       <c r="H34" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I34" t="inlineStr">
         <is>
@@ -1985,22 +1985,22 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D35" t="n">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E35" s="2" t="n">
         <v>32874</v>
       </c>
       <c r="F35" s="2" t="n">
-        <v>45017</v>
+        <v>45047</v>
       </c>
       <c r="G35" s="2" t="n">
         <v>35643</v>
       </c>
       <c r="H35" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I35" t="inlineStr">
         <is>
@@ -2033,7 +2033,7 @@
         <v>498</v>
       </c>
       <c r="D36" t="n">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="E36" s="2" t="n">
         <v>29952</v>
@@ -2045,7 +2045,7 @@
         <v>32813</v>
       </c>
       <c r="H36" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I36" t="inlineStr">
         <is>
@@ -2075,22 +2075,22 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="D37" t="n">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E37" s="2" t="n">
         <v>31048</v>
       </c>
       <c r="F37" s="2" t="n">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="G37" s="2" t="n">
         <v>35643</v>
       </c>
       <c r="H37" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I37" t="inlineStr">
         <is>
@@ -2120,22 +2120,22 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D38" t="n">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="E38" s="2" t="n">
         <v>34304</v>
       </c>
       <c r="F38" s="2" t="n">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="G38" s="2" t="n">
         <v>34121</v>
       </c>
       <c r="H38" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I38" t="inlineStr">
         <is>
@@ -2165,22 +2165,22 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D39" t="n">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E39" s="2" t="n">
         <v>38322</v>
       </c>
       <c r="F39" s="2" t="n">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="G39" s="2" t="n">
         <v>38504</v>
       </c>
       <c r="H39" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I39" t="inlineStr">
         <is>
@@ -2210,22 +2210,22 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D40" t="n">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E40" s="2" t="n">
         <v>36526</v>
       </c>
       <c r="F40" s="2" t="n">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="G40" s="2" t="n">
         <v>35643</v>
       </c>
       <c r="H40" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I40" t="inlineStr">
         <is>
@@ -2255,22 +2255,22 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="D41" t="n">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E41" s="2" t="n">
         <v>33239</v>
       </c>
       <c r="F41" s="2" t="n">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="G41" s="2" t="n">
         <v>35643</v>
       </c>
       <c r="H41" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I41" t="inlineStr">
         <is>
@@ -2303,7 +2303,7 @@
         <v>234</v>
       </c>
       <c r="D42" t="n">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E42" s="2" t="n">
         <v>37956</v>
@@ -2315,7 +2315,7 @@
         <v>37928</v>
       </c>
       <c r="H42" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I42" t="inlineStr">
         <is>
@@ -2345,22 +2345,22 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D43" t="n">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E43" s="2" t="n">
         <v>30834</v>
       </c>
       <c r="F43" s="2" t="n">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="G43" s="2" t="n">
         <v>35643</v>
       </c>
       <c r="H43" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I43" t="inlineStr">
         <is>
@@ -2393,7 +2393,7 @@
         <v>401</v>
       </c>
       <c r="D44" t="n">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E44" s="2" t="n">
         <v>32874</v>
@@ -2405,7 +2405,7 @@
         <v>35643</v>
       </c>
       <c r="H44" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I44" t="inlineStr">
         <is>
@@ -2438,7 +2438,7 @@
         <v>373</v>
       </c>
       <c r="D45" t="n">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E45" s="2" t="n">
         <v>33604</v>
@@ -2450,7 +2450,7 @@
         <v>35643</v>
       </c>
       <c r="H45" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I45" t="inlineStr">
         <is>
@@ -2480,22 +2480,22 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D46" t="n">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E46" s="2" t="n">
         <v>35065</v>
       </c>
       <c r="F46" s="2" t="n">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="G46" s="2" t="n">
         <v>36220</v>
       </c>
       <c r="H46" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I46" t="inlineStr">
         <is>
@@ -2525,22 +2525,22 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D47" t="n">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E47" s="2" t="n">
         <v>35034</v>
       </c>
       <c r="F47" s="2" t="n">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="G47" s="2" t="n">
         <v>37288</v>
       </c>
       <c r="H47" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I47" t="inlineStr">
         <is>
@@ -2570,22 +2570,22 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D48" t="n">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="E48" s="2" t="n">
         <v>34335</v>
       </c>
       <c r="F48" s="2" t="n">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="G48" s="2" t="n">
         <v>35643</v>
       </c>
       <c r="H48" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I48" t="inlineStr">
         <is>
@@ -2615,22 +2615,22 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D49" t="n">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E49" s="2" t="n">
         <v>36161</v>
       </c>
       <c r="F49" s="2" t="n">
-        <v>45017</v>
+        <v>45047</v>
       </c>
       <c r="G49" s="2" t="n">
         <v>35643</v>
       </c>
       <c r="H49" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I49" t="inlineStr">
         <is>
@@ -2660,22 +2660,22 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D50" t="n">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E50" s="2" t="n">
         <v>34304</v>
       </c>
       <c r="F50" s="2" t="n">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="G50" s="2" t="n">
         <v>36892</v>
       </c>
       <c r="H50" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I50" t="inlineStr">
         <is>
@@ -2708,19 +2708,19 @@
         <v>500</v>
       </c>
       <c r="D51" t="n">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E51" s="2" t="n">
-        <v>29646</v>
+        <v>29707</v>
       </c>
       <c r="F51" s="2" t="n">
-        <v>45017</v>
+        <v>45047</v>
       </c>
       <c r="G51" s="2" t="n">
         <v>35643</v>
       </c>
       <c r="H51" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I51" t="inlineStr">
         <is>
@@ -2753,7 +2753,7 @@
         <v>342</v>
       </c>
       <c r="D52" t="n">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="E52" s="2" t="n">
         <v>34700</v>
@@ -2765,7 +2765,7 @@
         <v>35643</v>
       </c>
       <c r="H52" s="2" t="n">
-        <v>45110</v>
+        <v>45139</v>
       </c>
       <c r="I52" t="inlineStr">
         <is>

</xml_diff>